<commit_message>
updated notebooks and control file to add extra variable EXTRA_DELTA_OUTFLOW_SELECTDV
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A02A88B-431A-4CEC-A7E6-2987840A4F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADB0EF7-E2DC-4AA8-8571-73D6C2E802E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12510" yWindow="-18345" windowWidth="17460" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Init" sheetId="1" r:id="rId1"/>
@@ -211,9 +211,6 @@
     <t>J18</t>
   </si>
   <si>
-    <t>E239</t>
-  </si>
-  <si>
     <t>Inflows Extraction Dir</t>
   </si>
   <si>
@@ -239,6 +236,9 @@
   </si>
   <si>
     <t>E220</t>
+  </si>
+  <si>
+    <t>E240</t>
   </si>
 </sst>
 </file>
@@ -578,7 +578,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -759,7 +759,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -826,26 +826,26 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -853,13 +853,13 @@
         <v>45</v>
       </c>
       <c r="B26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated init file CalSim3DataExtractionInitFile_v4.xlsx
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADB0EF7-E2DC-4AA8-8571-73D6C2E802E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FAE7406-5552-4B8B-B291-2B775D0CEF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12510" yWindow="-18345" windowWidth="17460" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8385" yWindow="-16050" windowWidth="29070" windowHeight="16470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Init" sheetId="1" r:id="rId1"/>
@@ -238,7 +238,7 @@
     <t>E220</t>
   </si>
   <si>
-    <t>E240</t>
+    <t>E242</t>
   </si>
 </sst>
 </file>
@@ -577,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
modified init file to extend to new scenario 19
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FAE7406-5552-4B8B-B291-2B775D0CEF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D42193-6ED7-4972-959B-347C5CB4422B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8385" yWindow="-16050" windowWidth="29070" windowHeight="16470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Init" sheetId="1" r:id="rId1"/>
@@ -190,27 +190,6 @@
     <t>trend_report_variables_v5.xlsx</t>
   </si>
   <si>
-    <t>A18</t>
-  </si>
-  <si>
-    <t>B18</t>
-  </si>
-  <si>
-    <t>C18</t>
-  </si>
-  <si>
-    <t>G18</t>
-  </si>
-  <si>
-    <t>H18</t>
-  </si>
-  <si>
-    <t>I18</t>
-  </si>
-  <si>
-    <t>J18</t>
-  </si>
-  <si>
     <t>Inflows Extraction Dir</t>
   </si>
   <si>
@@ -239,6 +218,27 @@
   </si>
   <si>
     <t>E242</t>
+  </si>
+  <si>
+    <t>A19</t>
+  </si>
+  <si>
+    <t>B19</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>G19</t>
+  </si>
+  <si>
+    <t>H19</t>
+  </si>
+  <si>
+    <t>I19</t>
+  </si>
+  <si>
+    <t>J19</t>
   </si>
 </sst>
 </file>
@@ -578,7 +578,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,7 +637,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -651,7 +651,7 @@
         <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -665,7 +665,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -679,7 +679,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -693,7 +693,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -707,7 +707,7 @@
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -721,7 +721,7 @@
         <v>37</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -759,7 +759,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -826,26 +826,26 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -853,13 +853,13 @@
         <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated init files to include scenario 20
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D42193-6ED7-4972-959B-347C5CB4422B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E97C5B-765C-49EF-971F-185DCA258925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Init" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -220,25 +221,25 @@
     <t>E242</t>
   </si>
   <si>
-    <t>A19</t>
-  </si>
-  <si>
-    <t>B19</t>
-  </si>
-  <si>
-    <t>C19</t>
-  </si>
-  <si>
-    <t>G19</t>
-  </si>
-  <si>
-    <t>H19</t>
-  </si>
-  <si>
-    <t>I19</t>
-  </si>
-  <si>
-    <t>J19</t>
+    <t>A120</t>
+  </si>
+  <si>
+    <t>B20</t>
+  </si>
+  <si>
+    <t>C20</t>
+  </si>
+  <si>
+    <t>G20</t>
+  </si>
+  <si>
+    <t>H20</t>
+  </si>
+  <si>
+    <t>I20</t>
+  </si>
+  <si>
+    <t>J20</t>
   </si>
 </sst>
 </file>
@@ -578,7 +579,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A5" sqref="A5:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated init files for scenario 21
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
@@ -3,15 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E97C5B-765C-49EF-971F-185DCA258925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA747963-BE72-410B-8297-8B9D5E46A7EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Init" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -221,25 +220,25 @@
     <t>E242</t>
   </si>
   <si>
-    <t>A120</t>
-  </si>
-  <si>
-    <t>B20</t>
-  </si>
-  <si>
-    <t>C20</t>
-  </si>
-  <si>
-    <t>G20</t>
-  </si>
-  <si>
-    <t>H20</t>
-  </si>
-  <si>
-    <t>I20</t>
-  </si>
-  <si>
-    <t>J20</t>
+    <t>A21</t>
+  </si>
+  <si>
+    <t>B21</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>G21</t>
+  </si>
+  <si>
+    <t>H21</t>
+  </si>
+  <si>
+    <t>I21</t>
+  </si>
+  <si>
+    <t>J21</t>
   </si>
 </sst>
 </file>
@@ -579,7 +578,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:D11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated files t include scenarios 22-24
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA747963-BE72-410B-8297-8B9D5E46A7EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7737B9EF-A9BD-4473-BAB4-49E765D41AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -220,25 +220,25 @@
     <t>E242</t>
   </si>
   <si>
-    <t>A21</t>
-  </si>
-  <si>
-    <t>B21</t>
-  </si>
-  <si>
-    <t>C21</t>
-  </si>
-  <si>
-    <t>G21</t>
-  </si>
-  <si>
-    <t>H21</t>
-  </si>
-  <si>
-    <t>I21</t>
-  </si>
-  <si>
-    <t>J21</t>
+    <t>A24</t>
+  </si>
+  <si>
+    <t>B24</t>
+  </si>
+  <si>
+    <t>C24</t>
+  </si>
+  <si>
+    <t>G24</t>
+  </si>
+  <si>
+    <t>H24</t>
+  </si>
+  <si>
+    <t>I24</t>
+  </si>
+  <si>
+    <t>J24</t>
   </si>
 </sst>
 </file>
@@ -578,7 +578,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D5" sqref="D5:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
modified to extract AWOANN vars
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7737B9EF-A9BD-4473-BAB4-49E765D41AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227CC6CE-C7B3-4208-835D-777C7DED279D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -217,9 +217,6 @@
     <t>E220</t>
   </si>
   <si>
-    <t>E242</t>
-  </si>
-  <si>
     <t>A24</t>
   </si>
   <si>
@@ -239,6 +236,9 @@
   </si>
   <si>
     <t>J24</t>
+  </si>
+  <si>
+    <t>E247</t>
   </si>
 </sst>
 </file>
@@ -578,7 +578,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,7 +637,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -651,7 +651,7 @@
         <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -665,7 +665,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -679,7 +679,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -693,7 +693,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -707,7 +707,7 @@
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -721,7 +721,7 @@
         <v>37</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -759,7 +759,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
new init for scenario 29
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
@@ -3,17 +3,28 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227CC6CE-C7B3-4208-835D-777C7DED279D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8D47D5-E647-4463-B13F-81295ECDD044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Init" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -217,28 +228,28 @@
     <t>E220</t>
   </si>
   <si>
-    <t>A24</t>
-  </si>
-  <si>
-    <t>B24</t>
-  </si>
-  <si>
-    <t>C24</t>
-  </si>
-  <si>
-    <t>G24</t>
-  </si>
-  <si>
-    <t>H24</t>
-  </si>
-  <si>
-    <t>I24</t>
-  </si>
-  <si>
-    <t>J24</t>
-  </si>
-  <si>
     <t>E247</t>
+  </si>
+  <si>
+    <t>A25</t>
+  </si>
+  <si>
+    <t>B25</t>
+  </si>
+  <si>
+    <t>C25</t>
+  </si>
+  <si>
+    <t>G25</t>
+  </si>
+  <si>
+    <t>H25</t>
+  </si>
+  <si>
+    <t>I25</t>
+  </si>
+  <si>
+    <t>J25</t>
   </si>
 </sst>
 </file>
@@ -578,7 +589,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,7 +648,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -651,7 +662,7 @@
         <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -665,7 +676,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -679,7 +690,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -693,7 +704,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -707,7 +718,7 @@
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -721,7 +732,7 @@
         <v>37</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -759,7 +770,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated init files for scenario 46
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8D47D5-E647-4463-B13F-81295ECDD044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7746851A-951E-4D56-B9FD-7847017B1CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2700" yWindow="-21720" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Init" sheetId="1" r:id="rId1"/>
@@ -231,25 +231,25 @@
     <t>E247</t>
   </si>
   <si>
-    <t>A25</t>
-  </si>
-  <si>
-    <t>B25</t>
-  </si>
-  <si>
-    <t>C25</t>
-  </si>
-  <si>
-    <t>G25</t>
-  </si>
-  <si>
-    <t>H25</t>
-  </si>
-  <si>
-    <t>I25</t>
-  </si>
-  <si>
-    <t>J25</t>
+    <t>A26</t>
+  </si>
+  <si>
+    <t>B26</t>
+  </si>
+  <si>
+    <t>C26</t>
+  </si>
+  <si>
+    <t>G26</t>
+  </si>
+  <si>
+    <t>H26</t>
+  </si>
+  <si>
+    <t>I26</t>
+  </si>
+  <si>
+    <t>J26</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
updated init files for scenarios 25 and 27
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7746851A-951E-4D56-B9FD-7847017B1CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655397E8-D1BD-4F16-B239-735D57B910AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2700" yWindow="-21720" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -231,25 +231,25 @@
     <t>E247</t>
   </si>
   <si>
-    <t>A26</t>
-  </si>
-  <si>
-    <t>B26</t>
-  </si>
-  <si>
-    <t>C26</t>
-  </si>
-  <si>
-    <t>G26</t>
-  </si>
-  <si>
-    <t>H26</t>
-  </si>
-  <si>
-    <t>I26</t>
-  </si>
-  <si>
-    <t>J26</t>
+    <t>A28</t>
+  </si>
+  <si>
+    <t>B28</t>
+  </si>
+  <si>
+    <t>C28</t>
+  </si>
+  <si>
+    <t>G28</t>
+  </si>
+  <si>
+    <t>H28</t>
+  </si>
+  <si>
+    <t>I28</t>
+  </si>
+  <si>
+    <t>J28</t>
   </si>
 </sst>
 </file>
@@ -589,7 +589,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated to include TUCP trigger variable
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655397E8-D1BD-4F16-B239-735D57B910AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6013A9A7-F079-4EC0-B5DF-9E79F65FF5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2700" yWindow="-21720" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="765" yWindow="-16095" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Init" sheetId="1" r:id="rId1"/>
@@ -228,9 +228,6 @@
     <t>E220</t>
   </si>
   <si>
-    <t>E247</t>
-  </si>
-  <si>
     <t>A28</t>
   </si>
   <si>
@@ -250,6 +247,9 @@
   </si>
   <si>
     <t>J28</t>
+  </si>
+  <si>
+    <t>E248</t>
   </si>
 </sst>
 </file>
@@ -589,7 +589,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -648,7 +648,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -662,7 +662,7 @@
         <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -676,7 +676,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -690,7 +690,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -704,7 +704,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -718,7 +718,7 @@
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -732,7 +732,7 @@
         <v>37</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -770,7 +770,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added stream gain variables
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6013A9A7-F079-4EC0-B5DF-9E79F65FF5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DEDAE5-1B1D-468F-BAF4-F2854E009595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="765" yWindow="-16095" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Init" sheetId="1" r:id="rId1"/>
@@ -249,7 +249,7 @@
     <t>J28</t>
   </si>
   <si>
-    <t>E248</t>
+    <t>E253</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
changed delivery indices, only affects delivery data extraction
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DEDAE5-1B1D-468F-BAF4-F2854E009595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9B9844-688F-4A56-884A-B4FAF376FDF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -153,9 +153,6 @@
     <t>SV Dss path names</t>
   </si>
   <si>
-    <t>cs3rpt2022_all_demand_units_v20250113.xlsx</t>
-  </si>
-  <si>
     <t>all_demand_units</t>
   </si>
   <si>
@@ -177,9 +174,6 @@
     <t>A2</t>
   </si>
   <si>
-    <t>O389</t>
-  </si>
-  <si>
     <t>DV DSS Path Indices</t>
   </si>
   <si>
@@ -250,6 +244,12 @@
   </si>
   <si>
     <t>E253</t>
+  </si>
+  <si>
+    <t>cs3rpt2022_all_demand_units_v20251130.xlsx</t>
+  </si>
+  <si>
+    <t>O391</t>
   </si>
 </sst>
 </file>
@@ -586,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,7 +599,7 @@
     <col min="3" max="5" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -613,7 +613,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -621,7 +621,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -629,7 +629,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -637,7 +637,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -648,24 +648,26 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -676,12 +678,13 @@
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
         <v>38</v>
@@ -690,12 +693,13 @@
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
         <v>39</v>
@@ -704,10 +708,11 @@
         <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -718,12 +723,13 @@
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -732,10 +738,11 @@
         <v>37</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -743,15 +750,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
@@ -759,7 +766,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -770,10 +777,10 @@
         <v>25</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -783,10 +790,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -807,70 +814,70 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
         <v>45</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="D22" s="2" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated init files up to scenario 56
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9B9844-688F-4A56-884A-B4FAF376FDF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516904BB-9BB1-4DE2-800A-5825447906AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="3228" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Init" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>Name or description</t>
   </si>
@@ -222,34 +222,37 @@
     <t>E220</t>
   </si>
   <si>
-    <t>A28</t>
-  </si>
-  <si>
-    <t>B28</t>
-  </si>
-  <si>
-    <t>C28</t>
-  </si>
-  <si>
-    <t>G28</t>
-  </si>
-  <si>
-    <t>H28</t>
-  </si>
-  <si>
-    <t>I28</t>
-  </si>
-  <si>
-    <t>J28</t>
-  </si>
-  <si>
-    <t>E253</t>
-  </si>
-  <si>
-    <t>cs3rpt2022_all_demand_units_v20251130.xlsx</t>
-  </si>
-  <si>
-    <t>O391</t>
+    <t>Inflow List Indices</t>
+  </si>
+  <si>
+    <t>cs3rpt2022_all_demand_units_v20251111.xlsx</t>
+  </si>
+  <si>
+    <t>O440</t>
+  </si>
+  <si>
+    <t>E258</t>
+  </si>
+  <si>
+    <t>A31</t>
+  </si>
+  <si>
+    <t>B31</t>
+  </si>
+  <si>
+    <t>C31</t>
+  </si>
+  <si>
+    <t>G31</t>
+  </si>
+  <si>
+    <t>H31</t>
+  </si>
+  <si>
+    <t>I31</t>
+  </si>
+  <si>
+    <t>J31</t>
   </si>
 </sst>
 </file>
@@ -589,7 +592,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D5" sqref="D5:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -648,7 +651,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -663,7 +666,7 @@
         <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -678,7 +681,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -693,7 +696,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -708,7 +711,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -723,7 +726,7 @@
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -738,7 +741,7 @@
         <v>37</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -777,7 +780,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -817,7 +820,7 @@
         <v>42</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -839,7 +842,7 @@
         <v>46</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -868,7 +871,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
updated init files up to scenario 63
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516904BB-9BB1-4DE2-800A-5825447906AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560BF887-26D0-4FC8-BD84-5CCFEADDD327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3228" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Init" sheetId="1" r:id="rId1"/>
@@ -234,25 +234,25 @@
     <t>E258</t>
   </si>
   <si>
-    <t>A31</t>
-  </si>
-  <si>
-    <t>B31</t>
-  </si>
-  <si>
-    <t>C31</t>
-  </si>
-  <si>
-    <t>G31</t>
-  </si>
-  <si>
-    <t>H31</t>
-  </si>
-  <si>
-    <t>I31</t>
-  </si>
-  <si>
-    <t>J31</t>
+    <t>A33</t>
+  </si>
+  <si>
+    <t>B33</t>
+  </si>
+  <si>
+    <t>C33</t>
+  </si>
+  <si>
+    <t>G33</t>
+  </si>
+  <si>
+    <t>H33</t>
+  </si>
+  <si>
+    <t>I33</t>
+  </si>
+  <si>
+    <t>J33</t>
   </si>
 </sst>
 </file>
@@ -591,7 +591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D5" sqref="D5:D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated extraction for more demands and deliveries
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560BF887-26D0-4FC8-BD84-5CCFEADDD327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2AD9CC-080C-40EB-AF14-E2DC7D9AA903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -228,9 +228,6 @@
     <t>cs3rpt2022_all_demand_units_v20251111.xlsx</t>
   </si>
   <si>
-    <t>O440</t>
-  </si>
-  <si>
     <t>E258</t>
   </si>
   <si>
@@ -253,6 +250,9 @@
   </si>
   <si>
     <t>J33</t>
+  </si>
+  <si>
+    <t>O475</t>
   </si>
 </sst>
 </file>
@@ -592,7 +592,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D11"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -651,7 +651,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -666,7 +666,7 @@
         <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -681,7 +681,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -696,7 +696,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -711,7 +711,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -726,7 +726,7 @@
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -741,7 +741,7 @@
         <v>37</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -780,7 +780,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -842,7 +842,7 @@
         <v>46</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated init files for extra scenarios (30,39,42)
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2AD9CC-080C-40EB-AF14-E2DC7D9AA903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E45B7B-A643-4B5E-A0CC-5A50D4116B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -231,28 +231,28 @@
     <t>E258</t>
   </si>
   <si>
-    <t>A33</t>
-  </si>
-  <si>
-    <t>B33</t>
-  </si>
-  <si>
-    <t>C33</t>
-  </si>
-  <si>
-    <t>G33</t>
-  </si>
-  <si>
-    <t>H33</t>
-  </si>
-  <si>
-    <t>I33</t>
-  </si>
-  <si>
-    <t>J33</t>
-  </si>
-  <si>
     <t>O475</t>
+  </si>
+  <si>
+    <t>A36</t>
+  </si>
+  <si>
+    <t>B36</t>
+  </si>
+  <si>
+    <t>C36</t>
+  </si>
+  <si>
+    <t>G36</t>
+  </si>
+  <si>
+    <t>H36</t>
+  </si>
+  <si>
+    <t>I36</t>
+  </si>
+  <si>
+    <t>J36</t>
   </si>
 </sst>
 </file>
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -651,7 +651,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -666,7 +666,7 @@
         <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -681,7 +681,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -696,7 +696,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -711,7 +711,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -726,7 +726,7 @@
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -741,7 +741,7 @@
         <v>37</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -842,7 +842,7 @@
         <v>46</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated init files for extra scenarios (40,41,42,44)
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E45B7B-A643-4B5E-A0CC-5A50D4116B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8904BB5A-98A0-425C-A3A6-C429F2EB54BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,6 +11,7 @@
     <sheet name="Init" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -234,25 +235,25 @@
     <t>O475</t>
   </si>
   <si>
-    <t>A36</t>
-  </si>
-  <si>
-    <t>B36</t>
-  </si>
-  <si>
-    <t>C36</t>
-  </si>
-  <si>
-    <t>G36</t>
-  </si>
-  <si>
-    <t>H36</t>
-  </si>
-  <si>
-    <t>I36</t>
-  </si>
-  <si>
-    <t>J36</t>
+    <t>A39</t>
+  </si>
+  <si>
+    <t>B39</t>
+  </si>
+  <si>
+    <t>C39</t>
+  </si>
+  <si>
+    <t>G39</t>
+  </si>
+  <si>
+    <t>H39</t>
+  </si>
+  <si>
+    <t>I39</t>
+  </si>
+  <si>
+    <t>J39</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
updated init files for extra scenarios (45)
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8904BB5A-98A0-425C-A3A6-C429F2EB54BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A394BC4-885A-4487-AFB1-447E922A4F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -235,25 +235,25 @@
     <t>O475</t>
   </si>
   <si>
-    <t>A39</t>
-  </si>
-  <si>
-    <t>B39</t>
-  </si>
-  <si>
-    <t>C39</t>
-  </si>
-  <si>
-    <t>G39</t>
-  </si>
-  <si>
-    <t>H39</t>
-  </si>
-  <si>
-    <t>I39</t>
-  </si>
-  <si>
-    <t>J39</t>
+    <t>B40</t>
+  </si>
+  <si>
+    <t>C40</t>
+  </si>
+  <si>
+    <t>G40</t>
+  </si>
+  <si>
+    <t>H40</t>
+  </si>
+  <si>
+    <t>I40</t>
+  </si>
+  <si>
+    <t>J40</t>
+  </si>
+  <si>
+    <t>A40</t>
   </si>
 </sst>
 </file>
@@ -652,7 +652,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -667,7 +667,7 @@
         <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -682,7 +682,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -697,7 +697,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -712,7 +712,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -727,7 +727,7 @@
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -742,7 +742,7 @@
         <v>37</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E11" s="2"/>
     </row>

</xml_diff>

<commit_message>
updated init files for extra scenarios (26,28,32)
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A394BC4-885A-4487-AFB1-447E922A4F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFFBF90-3A7D-4B1C-8BF8-AF49C0EB3D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -229,31 +229,31 @@
     <t>cs3rpt2022_all_demand_units_v20251111.xlsx</t>
   </si>
   <si>
-    <t>E258</t>
-  </si>
-  <si>
     <t>O475</t>
   </si>
   <si>
-    <t>B40</t>
-  </si>
-  <si>
-    <t>C40</t>
-  </si>
-  <si>
-    <t>G40</t>
-  </si>
-  <si>
-    <t>H40</t>
-  </si>
-  <si>
-    <t>I40</t>
-  </si>
-  <si>
-    <t>J40</t>
-  </si>
-  <si>
-    <t>A40</t>
+    <t>A43</t>
+  </si>
+  <si>
+    <t>B43</t>
+  </si>
+  <si>
+    <t>C43</t>
+  </si>
+  <si>
+    <t>G43</t>
+  </si>
+  <si>
+    <t>H43</t>
+  </si>
+  <si>
+    <t>I43</t>
+  </si>
+  <si>
+    <t>J43</t>
+  </si>
+  <si>
+    <t>E261</t>
   </si>
 </sst>
 </file>
@@ -593,7 +593,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,7 +652,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -781,7 +781,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -843,7 +843,7 @@
         <v>46</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated init files for extra scenarios (31,65,33)
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFFBF90-3A7D-4B1C-8BF8-AF49C0EB3D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B046A1E-B53D-4330-BC3C-87A7A335F574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -232,28 +232,28 @@
     <t>O475</t>
   </si>
   <si>
-    <t>A43</t>
-  </si>
-  <si>
-    <t>B43</t>
-  </si>
-  <si>
-    <t>C43</t>
-  </si>
-  <si>
-    <t>G43</t>
-  </si>
-  <si>
-    <t>H43</t>
-  </si>
-  <si>
-    <t>I43</t>
-  </si>
-  <si>
-    <t>J43</t>
-  </si>
-  <si>
     <t>E261</t>
+  </si>
+  <si>
+    <t>A46</t>
+  </si>
+  <si>
+    <t>B46</t>
+  </si>
+  <si>
+    <t>C46</t>
+  </si>
+  <si>
+    <t>G46</t>
+  </si>
+  <si>
+    <t>H46</t>
+  </si>
+  <si>
+    <t>I46</t>
+  </si>
+  <si>
+    <t>J46</t>
   </si>
 </sst>
 </file>
@@ -593,7 +593,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D5" sqref="D5:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,7 +652,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -667,7 +667,7 @@
         <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -682,7 +682,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -697,7 +697,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -712,7 +712,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -727,7 +727,7 @@
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -742,7 +742,7 @@
         <v>37</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -781,7 +781,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added more vaariables to data extraction
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v4.xlsx
@@ -3,15 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B046A1E-B53D-4330-BC3C-87A7A335F574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30EAF47-4D5A-4934-B553-AC074BCB798E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2700" yWindow="-21720" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Init" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -232,9 +231,6 @@
     <t>O475</t>
   </si>
   <si>
-    <t>E261</t>
-  </si>
-  <si>
     <t>A46</t>
   </si>
   <si>
@@ -254,6 +250,9 @@
   </si>
   <si>
     <t>J46</t>
+  </si>
+  <si>
+    <t>E265</t>
   </si>
 </sst>
 </file>
@@ -593,7 +592,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,7 +651,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -667,7 +666,7 @@
         <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -682,7 +681,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -697,7 +696,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -712,7 +711,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -727,7 +726,7 @@
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -742,7 +741,7 @@
         <v>37</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -781,7 +780,7 @@
         <v>25</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>